<commit_message>
Projeto modificaod conforme necessidade do usuario
</commit_message>
<xml_diff>
--- a/DesafioCucumberTravelPHP/src/main/resources/massaDadosExcel/Login.xlsx
+++ b/DesafioCucumberTravelPHP/src/main/resources/massaDadosExcel/Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JudrianideBrito\Desktop\PROJETO BRITO\CucumberPhpTravel\DesafioCucumberTravelPHP\src\main\resources\massaDadosExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B90B9B2-C985-4C86-A788-0F83730CE680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE67A8A9-47A9-47A8-95D7-04435B930675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{EA4B0455-F2DC-49B9-8A8B-FB03D8BCD24C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Email</t>
   </si>
@@ -99,12 +99,6 @@
     <t>linha8</t>
   </si>
   <si>
-    <t>JOÃO</t>
-  </si>
-  <si>
-    <t>SILVA</t>
-  </si>
-  <si>
     <t>BORRACHARIA DO ZE</t>
   </si>
   <si>
@@ -123,40 +117,16 @@
     <t>ludrian</t>
   </si>
   <si>
-    <t>judriani</t>
-  </si>
-  <si>
-    <t>hellen</t>
-  </si>
-  <si>
-    <t>eloa</t>
-  </si>
-  <si>
-    <t>aurea</t>
-  </si>
-  <si>
-    <t>cizzy</t>
-  </si>
-  <si>
-    <t>kassia</t>
-  </si>
-  <si>
-    <t>dimizy</t>
-  </si>
-  <si>
-    <t>leopoldo</t>
-  </si>
-  <si>
-    <t>dasfadsfdsf</t>
-  </si>
-  <si>
-    <t>dfdafdsfdf</t>
-  </si>
-  <si>
     <t>dfdafdaf</t>
   </si>
   <si>
     <t>BORRACHARIA DO Z</t>
+  </si>
+  <si>
+    <t>ESDSON</t>
+  </si>
+  <si>
+    <t>MARCANTE</t>
   </si>
 </sst>
 </file>
@@ -761,7 +731,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A4" sqref="A4:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,13 +744,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>0</v>
@@ -789,144 +759,56 @@
     </row>
     <row r="2" spans="1:5" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D11" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1">
@@ -935,16 +817,8 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{D5522F51-97E7-4937-A750-24C3B14FC997}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{DE7B2944-4944-4A65-816B-C19B6BEEEAAE}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{7D8809D5-1096-4A82-A0A2-ABFBBC2024AD}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{A6771FA3-0521-4AA5-AC69-D9A371849DF4}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{5C9AA257-DEFC-44CA-AF33-0114A5A992AF}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{E7014D23-8AA1-4C32-8B4B-58DA0725937E}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{98EC4030-4CA7-49A5-80AE-96566E01A8D1}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{49B25642-D0F4-4B24-B300-EFF2C63C0D02}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{5B61A04B-C145-4EBA-9DD9-AA322DFA13D4}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{736EC1AE-FA06-4B4D-8AE8-E8045FD0884B}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alterado estrutura do projeto seguindo boas praticas
</commit_message>
<xml_diff>
--- a/DesafioCucumberTravelPHP/src/main/resources/massaDadosExcel/Login.xlsx
+++ b/DesafioCucumberTravelPHP/src/main/resources/massaDadosExcel/Login.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JudrianideBrito\Desktop\PROJETO BRITO\CucumberPhpTravel\DesafioCucumberTravelPHP\src\main\resources\massaDadosExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE67A8A9-47A9-47A8-95D7-04435B930675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D05806-1E54-46DF-9EF1-7DF918DB699A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{EA4B0455-F2DC-49B9-8A8B-FB03D8BCD24C}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Email</t>
   </si>
@@ -99,12 +99,6 @@
     <t>linha8</t>
   </si>
   <si>
-    <t>BORRACHARIA DO ZE</t>
-  </si>
-  <si>
-    <t>DOZE@GMAIL.COM</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -114,26 +108,42 @@
     <t>Business Name</t>
   </si>
   <si>
-    <t>ludrian</t>
-  </si>
-  <si>
-    <t>dfdafdaf</t>
-  </si>
-  <si>
-    <t>BORRACHARIA DO Z</t>
-  </si>
-  <si>
-    <t>ESDSON</t>
-  </si>
-  <si>
-    <t>MARCANTE</t>
+    <t>executado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ludrian </t>
+  </si>
+  <si>
+    <t>Santos De Brito</t>
+  </si>
+  <si>
+    <t>ACAI DA HELLEN</t>
+  </si>
+  <si>
+    <t>ACAI@ACAI</t>
+  </si>
+  <si>
+    <t>Jubileu</t>
+  </si>
+  <si>
+    <t>Que não Leu</t>
+  </si>
+  <si>
+    <t>DindinMaisDindin</t>
+  </si>
+  <si>
+    <t>dindin@dindin</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,12 +183,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <color rgb="FF40C440"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -286,7 +290,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -300,11 +304,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -631,8 +632,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="77.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -728,95 +729,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C282549-DD10-4FA6-923A-97D265817811}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="5"/>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1">
     <sortCondition ref="A1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{D5522F51-97E7-4937-A750-24C3B14FC997}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{DE7B2944-4944-4A65-816B-C19B6BEEEAAE}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{DE7B2944-4944-4A65-816B-C19B6BEEEAAE}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{BEDBB422-2B6D-4A2B-8761-29CF8C8C59F7}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>